<commit_message>
add output dirctory -1
</commit_message>
<xml_diff>
--- a/smoothmodel_output/1+ 对比 Flyme/1+对比Flyme.xlsx
+++ b/smoothmodel_output/1+ 对比 Flyme/1+对比Flyme.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pyCode\SmoothModel\smoothmodel_output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pyCode\SmoothModel\smoothmodel_output\1+ 对比 Flyme\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="12615" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="12615"/>
   </bookViews>
   <sheets>
     <sheet name="概览" sheetId="2" r:id="rId1"/>
@@ -2587,24 +2587,6 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2643,6 +2625,24 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2803,7 +2803,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2841,9 +2840,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -2863,7 +2860,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2901,9 +2897,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -2978,7 +2972,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3109,7 +3102,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3186,11 +3178,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="94958672"/>
-        <c:axId val="94959232"/>
+        <c:axId val="310074384"/>
+        <c:axId val="310074944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="94958672"/>
+        <c:axId val="310074384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3233,7 +3225,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94959232"/>
+        <c:crossAx val="310074944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3241,7 +3233,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94959232"/>
+        <c:axId val="310074944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3292,7 +3284,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94958672"/>
+        <c:crossAx val="310074384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3306,7 +3298,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4896,11 +4887,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="94962592"/>
-        <c:axId val="94963152"/>
+        <c:axId val="310078304"/>
+        <c:axId val="310078864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="94962592"/>
+        <c:axId val="310078304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4957,7 +4948,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94963152"/>
+        <c:crossAx val="310078864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4965,7 +4956,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94963152"/>
+        <c:axId val="310078864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4975,7 +4966,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94962592"/>
+        <c:crossAx val="310078304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5799,11 +5790,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="259618240"/>
-        <c:axId val="259618800"/>
+        <c:axId val="310082224"/>
+        <c:axId val="310082784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="259618240"/>
+        <c:axId val="310082224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5860,7 +5851,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259618800"/>
+        <c:crossAx val="310082784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5868,7 +5859,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="259618800"/>
+        <c:axId val="310082784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5878,7 +5869,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="259618240"/>
+        <c:crossAx val="310082224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6694,11 +6685,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="259622160"/>
-        <c:axId val="259622720"/>
+        <c:axId val="310086144"/>
+        <c:axId val="310086704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="259622160"/>
+        <c:axId val="310086144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6755,7 +6746,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259622720"/>
+        <c:crossAx val="310086704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6763,7 +6754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="259622720"/>
+        <c:axId val="310086704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6773,7 +6764,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="259622160"/>
+        <c:crossAx val="310086144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11199,8 +11190,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -11231,7 +11222,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="70" t="s">
         <v>212</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -11251,7 +11242,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A5" s="58"/>
+      <c r="A5" s="71"/>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -11269,7 +11260,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A6" s="59"/>
+      <c r="A6" s="72"/>
       <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
@@ -11287,7 +11278,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="70" t="s">
         <v>213</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -11307,7 +11298,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A9" s="58"/>
+      <c r="A9" s="71"/>
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
@@ -11325,7 +11316,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A10" s="59"/>
+      <c r="A10" s="72"/>
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
@@ -11343,7 +11334,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="70" t="s">
         <v>214</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -11363,7 +11354,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A13" s="59"/>
+      <c r="A13" s="72"/>
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
@@ -12025,7 +12016,7 @@
       </c>
     </row>
     <row r="3" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B3" s="60">
+      <c r="B3" s="73">
         <v>1</v>
       </c>
       <c r="C3" s="43" t="s">
@@ -12063,7 +12054,7 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B4" s="61">
+      <c r="B4" s="74">
         <v>1</v>
       </c>
       <c r="C4" s="44" t="s">
@@ -12101,7 +12092,7 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B5" s="62">
+      <c r="B5" s="75">
         <v>1</v>
       </c>
       <c r="C5" s="45" t="s">
@@ -12139,7 +12130,7 @@
       </c>
     </row>
     <row r="6" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B6" s="60">
+      <c r="B6" s="73">
         <v>2</v>
       </c>
       <c r="C6" s="43" t="s">
@@ -12177,7 +12168,7 @@
       </c>
     </row>
     <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B7" s="61">
+      <c r="B7" s="74">
         <v>2</v>
       </c>
       <c r="C7" s="44" t="s">
@@ -12215,7 +12206,7 @@
       </c>
     </row>
     <row r="8" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B8" s="62">
+      <c r="B8" s="75">
         <v>2</v>
       </c>
       <c r="C8" s="45" t="s">
@@ -12253,7 +12244,7 @@
       </c>
     </row>
     <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B9" s="60">
+      <c r="B9" s="73">
         <v>3</v>
       </c>
       <c r="C9" s="43" t="s">
@@ -12291,7 +12282,7 @@
       </c>
     </row>
     <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B10" s="61">
+      <c r="B10" s="74">
         <v>3</v>
       </c>
       <c r="C10" s="44" t="s">
@@ -12329,7 +12320,7 @@
       </c>
     </row>
     <row r="11" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B11" s="62">
+      <c r="B11" s="75">
         <v>3</v>
       </c>
       <c r="C11" s="45" t="s">
@@ -12367,7 +12358,7 @@
       </c>
     </row>
     <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B12" s="60">
+      <c r="B12" s="73">
         <v>4</v>
       </c>
       <c r="C12" s="43" t="s">
@@ -12405,7 +12396,7 @@
       </c>
     </row>
     <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B13" s="61">
+      <c r="B13" s="74">
         <v>4</v>
       </c>
       <c r="C13" s="44" t="s">
@@ -12443,7 +12434,7 @@
       </c>
     </row>
     <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B14" s="62">
+      <c r="B14" s="75">
         <v>4</v>
       </c>
       <c r="C14" s="45" t="s">
@@ -12481,7 +12472,7 @@
       </c>
     </row>
     <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B15" s="60">
+      <c r="B15" s="73">
         <v>5</v>
       </c>
       <c r="C15" s="43" t="s">
@@ -12519,7 +12510,7 @@
       </c>
     </row>
     <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B16" s="61">
+      <c r="B16" s="74">
         <v>5</v>
       </c>
       <c r="C16" s="44" t="s">
@@ -12557,7 +12548,7 @@
       </c>
     </row>
     <row r="17" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B17" s="62">
+      <c r="B17" s="75">
         <v>5</v>
       </c>
       <c r="C17" s="45" t="s">
@@ -12595,7 +12586,7 @@
       </c>
     </row>
     <row r="18" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B18" s="60">
+      <c r="B18" s="73">
         <v>6</v>
       </c>
       <c r="C18" s="43" t="s">
@@ -12633,7 +12624,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B19" s="61">
+      <c r="B19" s="74">
         <v>6</v>
       </c>
       <c r="C19" s="44" t="s">
@@ -12671,7 +12662,7 @@
       </c>
     </row>
     <row r="20" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B20" s="62">
+      <c r="B20" s="75">
         <v>6</v>
       </c>
       <c r="C20" s="45" t="s">
@@ -12709,7 +12700,7 @@
       </c>
     </row>
     <row r="21" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B21" s="60">
+      <c r="B21" s="73">
         <v>7</v>
       </c>
       <c r="C21" s="43" t="s">
@@ -12747,7 +12738,7 @@
       </c>
     </row>
     <row r="22" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B22" s="61">
+      <c r="B22" s="74">
         <v>7</v>
       </c>
       <c r="C22" s="44" t="s">
@@ -12785,7 +12776,7 @@
       </c>
     </row>
     <row r="23" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B23" s="62">
+      <c r="B23" s="75">
         <v>7</v>
       </c>
       <c r="C23" s="45" t="s">
@@ -12823,7 +12814,7 @@
       </c>
     </row>
     <row r="24" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B24" s="60">
+      <c r="B24" s="73">
         <v>8</v>
       </c>
       <c r="C24" s="43" t="s">
@@ -12861,7 +12852,7 @@
       </c>
     </row>
     <row r="25" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B25" s="61">
+      <c r="B25" s="74">
         <v>8</v>
       </c>
       <c r="C25" s="44" t="s">
@@ -12899,7 +12890,7 @@
       </c>
     </row>
     <row r="26" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B26" s="62">
+      <c r="B26" s="75">
         <v>8</v>
       </c>
       <c r="C26" s="45" t="s">
@@ -12937,7 +12928,7 @@
       </c>
     </row>
     <row r="27" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B27" s="60">
+      <c r="B27" s="73">
         <v>9</v>
       </c>
       <c r="C27" s="43" t="s">
@@ -12975,7 +12966,7 @@
       </c>
     </row>
     <row r="28" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B28" s="61">
+      <c r="B28" s="74">
         <v>9</v>
       </c>
       <c r="C28" s="44" t="s">
@@ -13013,7 +13004,7 @@
       </c>
     </row>
     <row r="29" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B29" s="62">
+      <c r="B29" s="75">
         <v>9</v>
       </c>
       <c r="C29" s="45" t="s">
@@ -13051,7 +13042,7 @@
       </c>
     </row>
     <row r="30" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B30" s="60">
+      <c r="B30" s="73">
         <v>10</v>
       </c>
       <c r="C30" s="43" t="s">
@@ -13089,7 +13080,7 @@
       </c>
     </row>
     <row r="31" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B31" s="61">
+      <c r="B31" s="74">
         <v>10</v>
       </c>
       <c r="C31" s="44" t="s">
@@ -13127,7 +13118,7 @@
       </c>
     </row>
     <row r="32" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B32" s="62">
+      <c r="B32" s="75">
         <v>10</v>
       </c>
       <c r="C32" s="45" t="s">
@@ -13165,7 +13156,7 @@
       </c>
     </row>
     <row r="33" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B33" s="60">
+      <c r="B33" s="73">
         <v>11</v>
       </c>
       <c r="C33" s="43" t="s">
@@ -13203,7 +13194,7 @@
       </c>
     </row>
     <row r="34" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B34" s="61">
+      <c r="B34" s="74">
         <v>11</v>
       </c>
       <c r="C34" s="44" t="s">
@@ -13241,7 +13232,7 @@
       </c>
     </row>
     <row r="35" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B35" s="62">
+      <c r="B35" s="75">
         <v>11</v>
       </c>
       <c r="C35" s="45" t="s">
@@ -13279,7 +13270,7 @@
       </c>
     </row>
     <row r="36" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B36" s="60">
+      <c r="B36" s="73">
         <v>12</v>
       </c>
       <c r="C36" s="43" t="s">
@@ -13317,7 +13308,7 @@
       </c>
     </row>
     <row r="37" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B37" s="61">
+      <c r="B37" s="74">
         <v>12</v>
       </c>
       <c r="C37" s="44" t="s">
@@ -13355,7 +13346,7 @@
       </c>
     </row>
     <row r="38" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B38" s="62">
+      <c r="B38" s="75">
         <v>12</v>
       </c>
       <c r="C38" s="45" t="s">
@@ -13393,7 +13384,7 @@
       </c>
     </row>
     <row r="39" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B39" s="60">
+      <c r="B39" s="73">
         <v>13</v>
       </c>
       <c r="C39" s="43" t="s">
@@ -13431,7 +13422,7 @@
       </c>
     </row>
     <row r="40" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B40" s="61">
+      <c r="B40" s="74">
         <v>13</v>
       </c>
       <c r="C40" s="44" t="s">
@@ -13469,7 +13460,7 @@
       </c>
     </row>
     <row r="41" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B41" s="62">
+      <c r="B41" s="75">
         <v>13</v>
       </c>
       <c r="C41" s="45" t="s">
@@ -13507,7 +13498,7 @@
       </c>
     </row>
     <row r="42" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B42" s="60">
+      <c r="B42" s="73">
         <v>14</v>
       </c>
       <c r="C42" s="43" t="s">
@@ -13545,7 +13536,7 @@
       </c>
     </row>
     <row r="43" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B43" s="61">
+      <c r="B43" s="74">
         <v>14</v>
       </c>
       <c r="C43" s="44" t="s">
@@ -13583,7 +13574,7 @@
       </c>
     </row>
     <row r="44" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B44" s="62">
+      <c r="B44" s="75">
         <v>14</v>
       </c>
       <c r="C44" s="45" t="s">
@@ -13621,7 +13612,7 @@
       </c>
     </row>
     <row r="45" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B45" s="60">
+      <c r="B45" s="73">
         <v>15</v>
       </c>
       <c r="C45" s="43" t="s">
@@ -13659,7 +13650,7 @@
       </c>
     </row>
     <row r="46" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B46" s="61"/>
+      <c r="B46" s="74"/>
       <c r="C46" s="44" t="s">
         <v>53</v>
       </c>
@@ -13695,7 +13686,7 @@
       </c>
     </row>
     <row r="47" spans="2:13" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B47" s="62"/>
+      <c r="B47" s="75"/>
       <c r="C47" s="45" t="s">
         <v>53</v>
       </c>
@@ -13735,21 +13726,21 @@
     <sortCondition ref="B99"/>
   </sortState>
   <mergeCells count="15">
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B20"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14087,7 +14078,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B2:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -14137,34 +14128,34 @@
       <c r="B3" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="63" t="s">
         <v>196</v>
       </c>
-      <c r="D3" s="69">
+      <c r="D3" s="63">
         <v>10.09</v>
       </c>
-      <c r="E3" s="69">
+      <c r="E3" s="63">
         <v>9.93</v>
       </c>
-      <c r="F3" s="70">
+      <c r="F3" s="64">
         <v>0.59789999999999999</v>
       </c>
-      <c r="G3" s="70">
+      <c r="G3" s="64">
         <v>1.9699999999999999E-2</v>
       </c>
-      <c r="H3" s="71" t="s">
+      <c r="H3" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="71" t="s">
+      <c r="I3" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="71" t="s">
+      <c r="J3" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="K3" s="71" t="s">
+      <c r="K3" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="65" t="s">
         <v>59</v>
       </c>
     </row>
@@ -14172,69 +14163,69 @@
       <c r="B4" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="66" t="s">
         <v>194</v>
       </c>
-      <c r="D4" s="72">
+      <c r="D4" s="66">
         <v>11.02</v>
       </c>
-      <c r="E4" s="72">
+      <c r="E4" s="66">
         <v>10.62</v>
       </c>
-      <c r="F4" s="73">
+      <c r="F4" s="67">
         <v>50.08</v>
       </c>
-      <c r="G4" s="74">
+      <c r="G4" s="68">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="H4" s="75" t="s">
+      <c r="H4" s="69" t="s">
         <v>506</v>
       </c>
-      <c r="I4" s="75" t="s">
+      <c r="I4" s="69" t="s">
         <v>507</v>
       </c>
-      <c r="J4" s="75" t="s">
+      <c r="J4" s="69" t="s">
         <v>508</v>
       </c>
-      <c r="K4" s="75" t="s">
+      <c r="K4" s="69" t="s">
         <v>509</v>
       </c>
-      <c r="L4" s="75" t="s">
+      <c r="L4" s="69" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="D5" s="65">
+      <c r="D5" s="59">
         <v>14.59</v>
       </c>
-      <c r="E5" s="65">
+      <c r="E5" s="59">
         <v>14.42</v>
       </c>
-      <c r="F5" s="66">
+      <c r="F5" s="60">
         <v>0.23319999999999999</v>
       </c>
-      <c r="G5" s="66">
+      <c r="G5" s="60">
         <v>2.4199999999999999E-2</v>
       </c>
-      <c r="H5" s="67" t="s">
+      <c r="H5" s="61" t="s">
         <v>149</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="61" t="s">
         <v>150</v>
       </c>
-      <c r="J5" s="67" t="s">
+      <c r="J5" s="61" t="s">
         <v>151</v>
       </c>
-      <c r="K5" s="67" t="s">
+      <c r="K5" s="61" t="s">
         <v>152</v>
       </c>
-      <c r="L5" s="68" t="s">
+      <c r="L5" s="62" t="s">
         <v>153</v>
       </c>
     </row>
@@ -14554,7 +14545,7 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="73" t="s">
         <v>205</v>
       </c>
       <c r="C15" s="17" t="s">
@@ -14589,7 +14580,7 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="74" t="s">
         <v>78</v>
       </c>
       <c r="C16" s="14" t="s">
@@ -14624,7 +14615,7 @@
       </c>
     </row>
     <row r="17" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="75" t="s">
         <v>78</v>
       </c>
       <c r="C17" s="22" t="s">
@@ -14659,7 +14650,7 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="73" t="s">
         <v>209</v>
       </c>
       <c r="C18" s="17" t="s">
@@ -14694,7 +14685,7 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="74" t="s">
         <v>84</v>
       </c>
       <c r="C19" s="14" t="s">
@@ -14729,7 +14720,7 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="75" t="s">
         <v>84</v>
       </c>
       <c r="C20" s="22" t="s">
@@ -14764,7 +14755,7 @@
       </c>
     </row>
     <row r="21" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="73" t="s">
         <v>90</v>
       </c>
       <c r="C21" s="17" t="s">
@@ -14799,7 +14790,7 @@
       </c>
     </row>
     <row r="22" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="74" t="s">
         <v>90</v>
       </c>
       <c r="C22" s="14" t="s">
@@ -14834,7 +14825,7 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="75" t="s">
         <v>90</v>
       </c>
       <c r="C23" s="22" t="s">
@@ -14869,7 +14860,7 @@
       </c>
     </row>
     <row r="24" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="73" t="s">
         <v>96</v>
       </c>
       <c r="C24" s="17" t="s">
@@ -14904,7 +14895,7 @@
       </c>
     </row>
     <row r="25" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="74" t="s">
         <v>96</v>
       </c>
       <c r="C25" s="14" t="s">
@@ -14939,7 +14930,7 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="75" t="s">
         <v>96</v>
       </c>
       <c r="C26" s="22" t="s">
@@ -14974,7 +14965,7 @@
       </c>
     </row>
     <row r="27" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="73" t="s">
         <v>102</v>
       </c>
       <c r="C27" s="17" t="s">
@@ -15009,7 +15000,7 @@
       </c>
     </row>
     <row r="28" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="61" t="s">
+      <c r="B28" s="74" t="s">
         <v>102</v>
       </c>
       <c r="C28" s="14" t="s">
@@ -15044,7 +15035,7 @@
       </c>
     </row>
     <row r="29" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="75" t="s">
         <v>102</v>
       </c>
       <c r="C29" s="22" t="s">

</xml_diff>